<commit_message>
Modelo está rodando, com adoção negativa
</commit_message>
<xml_diff>
--- a/current_model/params.xlsx
+++ b/current_model/params.xlsx
@@ -444,7 +444,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +480,8 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>0.01</v>
+        <f>D2/3</f>
+        <v>3.3333333333333335E-3</v>
       </c>
       <c r="D2">
         <v>0.01</v>
@@ -497,7 +498,8 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>100</v>
+        <f t="shared" ref="C3:C6" si="0">D3/3</f>
+        <v>33.333333333333336</v>
       </c>
       <c r="D3">
         <v>100</v>
@@ -514,7 +516,8 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>0.02</v>
+        <f t="shared" si="0"/>
+        <v>6.6666666666666671E-3</v>
       </c>
       <c r="D4">
         <v>0.02</v>
@@ -531,7 +534,8 @@
         <v>17</v>
       </c>
       <c r="C5">
-        <v>100000</v>
+        <f t="shared" si="0"/>
+        <v>33333.333333333336</v>
       </c>
       <c r="D5">
         <v>100000</v>
@@ -548,7 +552,8 @@
         <v>18</v>
       </c>
       <c r="C6">
-        <v>100000</v>
+        <f t="shared" si="0"/>
+        <v>33333.333333333336</v>
       </c>
       <c r="D6">
         <v>100000</v>

</xml_diff>

<commit_message>
Modelo de Difusão Funcionando
</commit_message>
<xml_diff>
--- a/current_model/params.xlsx
+++ b/current_model/params.xlsx
@@ -443,9 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3AF1C2-6E06-403B-B596-52A55D7EBB3C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -480,8 +478,8 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <f>D2/3</f>
-        <v>3.3333333333333335E-3</v>
+        <f>D2/5</f>
+        <v>2E-3</v>
       </c>
       <c r="D2">
         <v>0.01</v>
@@ -498,8 +496,8 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C6" si="0">D3/3</f>
-        <v>33.333333333333336</v>
+        <f t="shared" ref="C3:C6" si="0">D3/5</f>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>100</v>
@@ -517,7 +515,7 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>6.6666666666666671E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D4">
         <v>0.02</v>
@@ -535,7 +533,7 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>33333.333333333336</v>
+        <v>20000</v>
       </c>
       <c r="D5">
         <v>100000</v>
@@ -553,7 +551,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>33333.333333333336</v>
+        <v>20000</v>
       </c>
       <c r="D6">
         <v>100000</v>

</xml_diff>

<commit_message>
Tentativas de corrigir o problema dos adopters negativos
</commit_message>
<xml_diff>
--- a/current_model/params.xlsx
+++ b/current_model/params.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Variavel</t>
   </si>
@@ -47,9 +47,6 @@
     <t>aTotalPopulation</t>
   </si>
   <si>
-    <t>siniPotentialAdopters</t>
-  </si>
-  <si>
     <t>Unidade</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
   </si>
   <si>
     <t>População Total</t>
-  </si>
-  <si>
-    <t>Consumidores Potenciais</t>
   </si>
 </sst>
 </file>
@@ -443,7 +437,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3AF1C2-6E06-403B-B596-52A55D7EBB3C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -458,7 +454,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -467,7 +463,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -475,17 +471,16 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <f>D2/5</f>
-        <v>2E-3</v>
+        <v>0.01</v>
       </c>
       <c r="D2">
         <v>0.01</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -493,17 +488,16 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C6" si="0">D3/5</f>
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D3">
         <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -511,17 +505,16 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>4.0000000000000001E-3</v>
+        <v>0.02</v>
       </c>
       <c r="D4">
         <v>0.02</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -529,32 +522,16 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>20000</v>
+        <v>1000000</v>
       </c>
       <c r="D5">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>20000</v>
-      </c>
-      <c r="D6">
-        <v>100000</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modelo difusao completo e rodando
</commit_message>
<xml_diff>
--- a/current_model/params.xlsx
+++ b/current_model/params.xlsx
@@ -438,7 +438,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,7 +477,7 @@
         <v>0.01</v>
       </c>
       <c r="D2">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -491,7 +491,7 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>100</v>
@@ -508,10 +508,10 @@
         <v>15</v>
       </c>
       <c r="C4">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="D4">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Organizando Localização das funções
</commit_message>
<xml_diff>
--- a/current_model/params.xlsx
+++ b/current_model/params.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{8C8B848D-7755-48BA-85DF-1CF1830EFE49}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{8C8B848D-7755-48BA-85DF-1CF1830EFE49}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
+    <sheet name="configs" sheetId="2" r:id="rId2"/>
+    <sheet name="VariableNames" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>Variavel</t>
   </si>
@@ -75,6 +77,93 @@
   </si>
   <si>
     <t>População Total</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>ChartName</t>
+  </si>
+  <si>
+    <t>TextName</t>
+  </si>
+  <si>
+    <t>Tempo</t>
+  </si>
+  <si>
+    <t>PotentialAdopters</t>
+  </si>
+  <si>
+    <t>Adopters</t>
+  </si>
+  <si>
+    <t>AdvEffectiveness</t>
+  </si>
+  <si>
+    <t>ModelName</t>
+  </si>
+  <si>
+    <t>ResultName</t>
+  </si>
+  <si>
+    <t>ContactRate</t>
+  </si>
+  <si>
+    <t>AdoptionFraction</t>
+  </si>
+  <si>
+    <t>TotalPopulation</t>
+  </si>
+  <si>
+    <t>Adoption_From_Advertising</t>
+  </si>
+  <si>
+    <t>Adoption_From_Word_of_Mouth</t>
+  </si>
+  <si>
+    <t>Adoption_Rate</t>
+  </si>
+  <si>
+    <t>Replicacao</t>
+  </si>
+  <si>
+    <t>EquationName</t>
+  </si>
+  <si>
+    <t>Clientes Potenciais</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>Efetividade do Anúncio</t>
+  </si>
+  <si>
+    <t>Taxa de Contato</t>
+  </si>
+  <si>
+    <t>Taxa de Adoção</t>
+  </si>
+  <si>
+    <t>Novos Clientes em Propaganda</t>
+  </si>
+  <si>
+    <t>Novos Clientes por Boca a Boca</t>
+  </si>
+  <si>
+    <t>Taxa de novos Clientes</t>
+  </si>
+  <si>
+    <t>Replicação</t>
+  </si>
+  <si>
+    <t>Anos</t>
   </si>
 </sst>
 </file>
@@ -437,9 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3AF1C2-6E06-403B-B596-52A55D7EBB3C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -541,4 +628,199 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5C43C2-1FAB-479F-820C-4D2F1DEEC0BC}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2015</v>
+      </c>
+      <c r="B2">
+        <v>2025</v>
+      </c>
+      <c r="C2">
+        <v>0.125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC23235-B0D4-47B4-91CF-02E948D7C177}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mais alterações, tentando rodar o PRIM com o OpenMORDM
</commit_message>
<xml_diff>
--- a/current_model/params.xlsx
+++ b/current_model/params.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{8C8B848D-7755-48BA-85DF-1CF1830EFE49}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3" xr2:uid="{8C8B848D-7755-48BA-85DF-1CF1830EFE49}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
     <sheet name="configs" sheetId="2" r:id="rId2"/>
     <sheet name="VariableNames" sheetId="3" r:id="rId3"/>
+    <sheet name="levers" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t>Variavel</t>
   </si>
@@ -164,6 +165,15 @@
   </si>
   <si>
     <t>Anos</t>
+  </si>
+  <si>
+    <t>Parametro1</t>
+  </si>
+  <si>
+    <t>Parametro2</t>
+  </si>
+  <si>
+    <t>Lever</t>
   </si>
 </sst>
 </file>
@@ -207,9 +217,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EC23235-B0D4-47B4-91CF-02E948D7C177}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,4 +834,77 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15055839-DAEF-45EB-940F-B4DD495D311F}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>